<commit_message>
add to fortune bag
</commit_message>
<xml_diff>
--- a/rpg-fortune-bag/checklist.xlsx
+++ b/rpg-fortune-bag/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/rpg-fortune-bag/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE0173B5-6EF9-A64B-8DCE-D0837AA62B54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4651BCE0-E0F1-C14A-B9A5-F967BD405C1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="460" windowWidth="26740" windowHeight="15780" xr2:uid="{1E5789D5-2688-9A4F-A034-5FEEFEB422BE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>year</t>
   </si>
@@ -84,6 +84,18 @@
   </si>
   <si>
     <t>RPG Fortune Bag '96</t>
+  </si>
+  <si>
+    <t>TRPGスーパーセッション大饗宴</t>
+  </si>
+  <si>
+    <t>RPG Super Session Feast</t>
+  </si>
+  <si>
+    <t>Enterbrain</t>
+  </si>
+  <si>
+    <t>rpg_super_session_feast.jpg</t>
   </si>
 </sst>
 </file>
@@ -450,17 +462,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6DD26AC-5363-A741-B69A-65F0535F20D2}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.5" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -540,6 +553,26 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2002</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>